<commit_message>
Add a new graphic
</commit_message>
<xml_diff>
--- a/data/schoolchoicepopularity_education_next/EdNext_SchoolChoice (Autosaved).xlsx
+++ b/data/schoolchoicepopularity_education_next/EdNext_SchoolChoice (Autosaved).xlsx
@@ -19,7 +19,6 @@
     <sheet name="2018 only" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -820,11 +819,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="530562200"/>
-        <c:axId val="530564160"/>
+        <c:axId val="319951432"/>
+        <c:axId val="319952216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="530562200"/>
+        <c:axId val="319951432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,7 +866,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530564160"/>
+        <c:crossAx val="319952216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -875,7 +874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="530564160"/>
+        <c:axId val="319952216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +982,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530562200"/>
+        <c:crossAx val="319951432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1380,11 +1379,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="530559064"/>
-        <c:axId val="530563376"/>
+        <c:axId val="319951824"/>
+        <c:axId val="319950256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="530559064"/>
+        <c:axId val="319951824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1427,7 +1426,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530563376"/>
+        <c:crossAx val="319950256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1435,7 +1434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="530563376"/>
+        <c:axId val="319950256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,7 +1485,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530559064"/>
+        <c:crossAx val="319951824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1965,11 +1964,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="530560632"/>
-        <c:axId val="530559456"/>
+        <c:axId val="322636216"/>
+        <c:axId val="322642096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="530560632"/>
+        <c:axId val="322636216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2012,7 +2011,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530559456"/>
+        <c:crossAx val="322642096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2020,7 +2019,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="530559456"/>
+        <c:axId val="322642096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530560632"/>
+        <c:crossAx val="322636216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2525,11 +2524,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="530564552"/>
-        <c:axId val="530560240"/>
+        <c:axId val="322638176"/>
+        <c:axId val="322639352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="530564552"/>
+        <c:axId val="322638176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2572,7 +2571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530560240"/>
+        <c:crossAx val="322639352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2580,7 +2579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="530560240"/>
+        <c:axId val="322639352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -2687,7 +2686,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530564552"/>
+        <c:crossAx val="322638176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3327,11 +3326,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="235178816"/>
-        <c:axId val="235176464"/>
+        <c:axId val="322635432"/>
+        <c:axId val="322640136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="235178816"/>
+        <c:axId val="322635432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3374,7 +3373,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235176464"/>
+        <c:crossAx val="322640136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3382,7 +3381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235176464"/>
+        <c:axId val="322640136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3490,7 +3489,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235178816"/>
+        <c:crossAx val="322635432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3593,7 +3592,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3606,25 +3605,40 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>School</a:t>
+              <a:rPr lang="en-US" sz="2400" b="1"/>
+              <a:t>Majority of Blacks, Hispanics Favor</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> Choice Support Strongest among Hispanics; </a:t>
+              <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="1"/>
+              <a:t>Vouchers</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
+              <a:t> </a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
             </a:br>
             <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t>Teachers Notably Less Enthused</a:t>
+              <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
+              <a:t>but Support for School Choice is Limited Overall</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
+            <a:endParaRPr lang="en-US" sz="2400" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.4283816599353212E-2"/>
+          <c:y val="4.1761368307239657E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3638,7 +3652,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3656,7 +3670,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13523675566799764"/>
+          <c:y val="0.23139133314595262"/>
+          <c:w val="0.8342222071888642"/>
+          <c:h val="0.69402774852672566"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
@@ -3685,11 +3709,108 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="50000"/>
+                    <a:alpha val="81000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:gradFill>
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="5000"/>
+                        <a:lumOff val="95000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="74000">
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="45000"/>
+                        <a:lumOff val="55000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="83000">
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="45000"/>
+                        <a:lumOff val="55000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="30000"/>
+                        <a:lumOff val="70000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="1"/>
+                </a:gradFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$6:$B$15</c:f>
+              <c:f>'2018 only'!$A$6:$B$13</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Charters</c:v>
@@ -3715,12 +3836,6 @@
                   <c:pt idx="7">
                     <c:v>Vouchers</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Charters</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Vouchers</c:v>
-                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3735,19 +3850,16 @@
                   <c:pt idx="6">
                     <c:v>White</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2018 only'!$C$6:$C$15</c:f>
+              <c:f>'2018 only'!$C$6:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -3771,12 +3883,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3806,11 +3912,75 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$6:$B$15</c:f>
+              <c:f>'2018 only'!$A$6:$B$13</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Charters</c:v>
@@ -3836,12 +4006,6 @@
                   <c:pt idx="7">
                     <c:v>Vouchers</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Charters</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Vouchers</c:v>
-                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3856,19 +4020,16 @@
                   <c:pt idx="6">
                     <c:v>White</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2018 only'!$D$6:$D$15</c:f>
+              <c:f>'2018 only'!$D$6:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>29</c:v>
                 </c:pt>
@@ -3892,12 +4053,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3929,9 +4084,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$6:$B$15</c:f>
+              <c:f>'2018 only'!$A$6:$B$13</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Charters</c:v>
@@ -3957,12 +4112,6 @@
                   <c:pt idx="7">
                     <c:v>Vouchers</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Charters</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Vouchers</c:v>
-                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3977,19 +4126,16 @@
                   <c:pt idx="6">
                     <c:v>White</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2018 only'!$E$6:$E$15</c:f>
+              <c:f>'2018 only'!$E$6:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>21</c:v>
                 </c:pt>
@@ -4013,12 +4159,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4052,9 +4192,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$6:$B$15</c:f>
+              <c:f>'2018 only'!$A$6:$B$13</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Charters</c:v>
@@ -4080,12 +4220,6 @@
                   <c:pt idx="7">
                     <c:v>Vouchers</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Charters</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Vouchers</c:v>
-                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4100,19 +4234,16 @@
                   <c:pt idx="6">
                     <c:v>White</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2018 only'!$F$6:$F$15</c:f>
+              <c:f>'2018 only'!$F$6:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>14</c:v>
                 </c:pt>
@@ -4136,12 +4267,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4175,9 +4300,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$6:$B$15</c:f>
+              <c:f>'2018 only'!$A$6:$B$13</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Charters</c:v>
@@ -4203,12 +4328,6 @@
                   <c:pt idx="7">
                     <c:v>Vouchers</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Charters</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Vouchers</c:v>
-                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4223,19 +4342,16 @@
                   <c:pt idx="6">
                     <c:v>White</c:v>
                   </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2018 only'!$G$6:$G$15</c:f>
+              <c:f>'2018 only'!$G$6:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>21</c:v>
                 </c:pt>
@@ -4258,12 +4374,6 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -4280,13 +4390,13 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="235174112"/>
-        <c:axId val="235175288"/>
+        <c:axId val="322637392"/>
+        <c:axId val="322635040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235174112"/>
+        <c:axId val="322637392"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4312,7 +4422,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4327,7 +4437,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235175288"/>
+        <c:crossAx val="322635040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4335,12 +4445,13 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235175288"/>
+        <c:axId val="322635040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4371,7 +4482,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4386,7 +4497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235174112"/>
+        <c:crossAx val="322637392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4400,7 +4511,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.4448145700073556E-2"/>
+          <c:y val="0.92774105033333276"/>
+          <c:w val="0.89999994171250974"/>
+          <c:h val="5.3305880401158377E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4414,7 +4534,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4454,7 +4574,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -8119,16 +8239,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>766536</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>168275</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>335643</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>517980</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9293,10 +9413,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="84" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -9308,12 +9428,12 @@
     <col min="7" max="7" width="23.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -9321,8 +9441,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="5" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="5" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="13" t="s">
         <v>26</v>
       </c>
@@ -9345,7 +9465,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
@@ -9367,8 +9487,12 @@
       <c r="G6" s="23">
         <v>21</v>
       </c>
+      <c r="H6">
+        <f>SUM(C6:D6)</f>
+        <v>44</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="19"/>
       <c r="B7" s="20" t="s">
         <v>24</v>
@@ -9388,8 +9512,12 @@
       <c r="G7" s="21">
         <v>12</v>
       </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H15" si="0">SUM(C7:D7)</f>
+        <v>44</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13" t="s">
         <v>33</v>
       </c>
@@ -9411,8 +9539,12 @@
       <c r="G8" s="23">
         <v>28</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="19"/>
       <c r="B9" s="20" t="s">
         <v>24</v>
@@ -9432,8 +9564,12 @@
       <c r="G9" s="21">
         <v>20</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="13" t="s">
         <v>34</v>
       </c>
@@ -9455,8 +9591,12 @@
       <c r="G10" s="23">
         <v>18</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="19"/>
       <c r="B11" s="20" t="s">
         <v>24</v>
@@ -9476,8 +9616,12 @@
       <c r="G11" s="21">
         <v>10</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="13" t="s">
         <v>32</v>
       </c>
@@ -9499,8 +9643,12 @@
       <c r="G12" s="23">
         <v>20</v>
       </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A13" s="19"/>
       <c r="B13" s="20" t="s">
         <v>24</v>
@@ -9520,8 +9668,12 @@
       <c r="G13" s="21">
         <v>11</v>
       </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="16" t="s">
         <v>8</v>
       </c>
@@ -9543,8 +9695,12 @@
       <c r="G14" s="18">
         <v>12</v>
       </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="19"/>
       <c r="B15" s="20" t="s">
         <v>24</v>
@@ -9563,6 +9719,10 @@
       </c>
       <c r="G15" s="21">
         <v>11</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>